<commit_message>
Technology list with insert queries Scripts
</commit_message>
<xml_diff>
--- a/DocumentsAndScripts/Technology List.xlsx
+++ b/DocumentsAndScripts/Technology List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venroja\source\repos\sateeshmunagala\nopCommerce\DocumentsAndScripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55BEF05-3CB9-4A08-B1A1-7689B98B5A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506C9775-1680-400D-ADA2-FFE2EB344513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -899,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G165"/>
+  <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="C142" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -912,14 +912,15 @@
     <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="128.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>94</v>
       </c>
@@ -939,8 +940,12 @@
       <c r="G2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H2" t="str">
+        <f>_xlfn.CONCAT(C2,D2,E2,F2,G2)</f>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' AI', 7, 0);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>96</v>
       </c>
@@ -960,8 +965,12 @@
       <c r="G3" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H66" si="1">_xlfn.CONCAT(C3,D3,E3,F3,G3)</f>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' Android', 7, 1);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>55</v>
       </c>
@@ -981,8 +990,12 @@
       <c r="G4" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H4" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' Angular ', 7, 2);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>114</v>
       </c>
@@ -1002,8 +1015,12 @@
       <c r="G5" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H5" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' Appian Developer', 7, 3);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
@@ -1023,8 +1040,12 @@
       <c r="G6" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' AWS ', 7, 4);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>144</v>
       </c>
@@ -1044,8 +1065,12 @@
       <c r="G7" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H7" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' Big Data', 7, 5);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>49</v>
       </c>
@@ -1065,8 +1090,12 @@
       <c r="G8" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H8" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' Blockchain ', 7, 6);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>50</v>
       </c>
@@ -1086,8 +1115,12 @@
       <c r="G9" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H9" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' Cyber Ark ', 7, 7);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>111</v>
       </c>
@@ -1107,8 +1140,12 @@
       <c r="G10" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H10" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' Cyber Security ', 7, 8);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>113</v>
       </c>
@@ -1128,8 +1165,12 @@
       <c r="G11" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H11" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' Data Science', 7, 9);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>38</v>
       </c>
@@ -1149,8 +1190,12 @@
       <c r="G12" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H12" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' Dell Boomi ', 7, 10);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
@@ -1170,8 +1215,12 @@
       <c r="G13" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H13" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' DevOps ', 7, 11);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
@@ -1191,8 +1240,12 @@
       <c r="G14" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H14" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' DOT NET ', 7, 12);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -1212,8 +1265,12 @@
       <c r="G15" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H15" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' GIS ', 7, 13);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>112</v>
       </c>
@@ -1233,8 +1290,12 @@
       <c r="G16" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H16" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' Guidewire', 7, 14);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>73</v>
       </c>
@@ -1254,8 +1315,12 @@
       <c r="G17" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H17" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' MS sql server', 7, 15);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>110</v>
       </c>
@@ -1275,8 +1340,12 @@
       <c r="G18" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H18" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' Office 365 Admin', 7, 16);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
@@ -1296,8 +1365,12 @@
       <c r="G19" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H19" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' OKTA ', 7, 17);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>72</v>
       </c>
@@ -1317,8 +1390,12 @@
       <c r="G20" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H20" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' ORACLE', 7, 18);</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>45</v>
       </c>
@@ -1338,8 +1415,12 @@
       <c r="G21" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H21" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' Pega ', 7, 19);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
@@ -1359,8 +1440,12 @@
       <c r="G22" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H22" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' Performance Testing ', 7, 20);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>51</v>
       </c>
@@ -1380,8 +1465,12 @@
       <c r="G23" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H23" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' Power BI ', 7, 21);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>41</v>
       </c>
@@ -1401,8 +1490,12 @@
       <c r="G24" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H24" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' Python ', 7, 22);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>60</v>
       </c>
@@ -1422,8 +1515,12 @@
       <c r="G25" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H25" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' React js ', 7, 23);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>33</v>
       </c>
@@ -1443,8 +1540,12 @@
       <c r="G26" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H26" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' Salesforce ', 7, 24);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>39</v>
       </c>
@@ -1464,8 +1565,12 @@
       <c r="G27" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H27" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' SAP Hybris ', 7, 25);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>47</v>
       </c>
@@ -1485,8 +1590,12 @@
       <c r="G28" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H28" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' SAP Modules ', 7, 26);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>43</v>
       </c>
@@ -1506,8 +1615,12 @@
       <c r="G29" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H29" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' SAS ', 7, 27);</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>46</v>
       </c>
@@ -1527,8 +1640,12 @@
       <c r="G30" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H30" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' SCCM ', 7, 28);</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>48</v>
       </c>
@@ -1548,8 +1665,12 @@
       <c r="G31" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H31" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' SCRUM Master ', 7, 29);</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>56</v>
       </c>
@@ -1569,8 +1690,12 @@
       <c r="G32" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H32" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' Splunk ', 7, 30);</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>124</v>
       </c>
@@ -1590,8 +1715,12 @@
       <c r="G33" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H33" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' Talend', 7, 31);</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>52</v>
       </c>
@@ -1611,8 +1740,12 @@
       <c r="G34" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H34" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' TOSCA ', 7, 32);</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>31</v>
       </c>
@@ -1632,8 +1765,12 @@
       <c r="G35" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H35" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' UI/UX Developer ', 7, 33);</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>53</v>
       </c>
@@ -1653,8 +1790,12 @@
       <c r="G36" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H36" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' Workday ', 7, 34);</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>66</v>
       </c>
@@ -1674,8 +1815,12 @@
       <c r="G37" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H37" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' AutoML ', 7, 35);</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>63</v>
       </c>
@@ -1695,8 +1840,12 @@
       <c r="G38" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H38" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' BigQuery ', 7, 36);</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>65</v>
       </c>
@@ -1716,8 +1865,12 @@
       <c r="G39" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H39" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' DataFusion  ', 7, 37);</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>64</v>
       </c>
@@ -1737,8 +1890,12 @@
       <c r="G40" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H40" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' DataProc ', 7, 38);</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>54</v>
       </c>
@@ -1758,8 +1915,12 @@
       <c r="G41" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H41" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' Microstrategy ', 7, 39);</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>57</v>
       </c>
@@ -1779,8 +1940,12 @@
       <c r="G42" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H42" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' PostgreSql ', 7, 40);</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>58</v>
       </c>
@@ -1800,8 +1965,12 @@
       <c r="G43" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H43" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' Powershell Scripting ', 7, 41);</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>30</v>
       </c>
@@ -1821,8 +1990,12 @@
       <c r="G44" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H44" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' Servicenow ', 7, 42);</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>35</v>
       </c>
@@ -1842,8 +2015,12 @@
       <c r="G45" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H45" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' SnowFlake ', 7, 43);</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>40</v>
       </c>
@@ -1863,8 +2040,12 @@
       <c r="G46" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H46" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES (' Vmware Adminstartion ', 7, 44);</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>87</v>
       </c>
@@ -1884,8 +2065,12 @@
       <c r="G47" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H47" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Abinitio', 7, 45);</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>121</v>
       </c>
@@ -1905,8 +2090,12 @@
       <c r="G48" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H48" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Agile', 7, 46);</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>70</v>
       </c>
@@ -1926,8 +2115,12 @@
       <c r="G49" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H49" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('AirFlow', 7, 47);</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>155</v>
       </c>
@@ -1947,8 +2140,12 @@
       <c r="G50" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H50" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Asp.Net Core', 7, 48);</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>118</v>
       </c>
@@ -1968,8 +2165,12 @@
       <c r="G51" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H51" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Athena', 7, 49);</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>132</v>
       </c>
@@ -1989,8 +2190,12 @@
       <c r="G52" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H52" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('AWS Cloud Engineer', 7, 50);</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>13</v>
       </c>
@@ -2010,8 +2215,12 @@
       <c r="G53" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H53" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('AWS, ', 7, 51);</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>136</v>
       </c>
@@ -2031,8 +2240,12 @@
       <c r="G54" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H54" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('AWS-Athena ', 7, 52);</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>134</v>
       </c>
@@ -2052,8 +2265,12 @@
       <c r="G55" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H55" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('AWS-EC2', 7, 53);</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>135</v>
       </c>
@@ -2073,8 +2290,12 @@
       <c r="G56" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H56" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('AWS-Glue ', 7, 54);</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>138</v>
       </c>
@@ -2094,8 +2315,12 @@
       <c r="G57" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H57" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('AWS-IAM  ', 7, 55);</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>137</v>
       </c>
@@ -2115,8 +2340,12 @@
       <c r="G58" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H58" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('AWS-RDS  ', 7, 56);</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>133</v>
       </c>
@@ -2136,8 +2365,12 @@
       <c r="G59" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H59" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('AWS-S3', 7, 57);</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>98</v>
       </c>
@@ -2157,8 +2390,12 @@
       <c r="G60" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H60" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Azure', 7, 58);</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>90</v>
       </c>
@@ -2178,8 +2415,12 @@
       <c r="G61" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H61" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Azure Data Factory', 7, 59);</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>62</v>
       </c>
@@ -2199,8 +2440,12 @@
       <c r="G62" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H62" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Azure Devops ', 7, 60);</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>23</v>
       </c>
@@ -2220,8 +2465,12 @@
       <c r="G63" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H63" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Bigdata', 7, 61);</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>120</v>
       </c>
@@ -2241,8 +2490,12 @@
       <c r="G64" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H64" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Bit Bucket', 7, 62);</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>0</v>
       </c>
@@ -2262,8 +2515,12 @@
       <c r="G65" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H65" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Blue prism  ', 7, 63);</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>151</v>
       </c>
@@ -2283,8 +2540,12 @@
       <c r="G66" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H66" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Bootstrap', 7, 64);</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>148</v>
       </c>
@@ -2292,7 +2553,7 @@
         <v>107</v>
       </c>
       <c r="D67" t="str">
-        <f t="shared" ref="D67:D130" si="1">A67</f>
+        <f t="shared" ref="D67:D130" si="2">A67</f>
         <v>C#</v>
       </c>
       <c r="E67" t="s">
@@ -2304,8 +2565,12 @@
       <c r="G67" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H67" t="str">
+        <f t="shared" ref="H67:H130" si="3">_xlfn.CONCAT(C67,D67,E67,F67,G67)</f>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('C#', 7, 65);</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>147</v>
       </c>
@@ -2313,7 +2578,7 @@
         <v>107</v>
       </c>
       <c r="D68" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>C++</v>
       </c>
       <c r="E68" t="s">
@@ -2325,8 +2590,12 @@
       <c r="G68" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H68" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('C++', 7, 66);</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>4</v>
       </c>
@@ -2334,7 +2603,7 @@
         <v>107</v>
       </c>
       <c r="D69" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Check Point </v>
       </c>
       <c r="E69" t="s">
@@ -2346,8 +2615,12 @@
       <c r="G69" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H69" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Check Point ', 7, 67);</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>16</v>
       </c>
@@ -2355,7 +2628,7 @@
         <v>107</v>
       </c>
       <c r="D70" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Citrix</v>
       </c>
       <c r="E70" t="s">
@@ -2367,8 +2640,12 @@
       <c r="G70" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H70" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Citrix', 7, 68);</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>81</v>
       </c>
@@ -2376,7 +2653,7 @@
         <v>107</v>
       </c>
       <c r="D71" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Cloud Data Store </v>
       </c>
       <c r="E71" t="s">
@@ -2388,8 +2665,12 @@
       <c r="G71" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H71" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Cloud Data Store ', 7, 69);</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>7</v>
       </c>
@@ -2397,7 +2678,7 @@
         <v>107</v>
       </c>
       <c r="D72" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>CloudERA </v>
       </c>
       <c r="E72" t="s">
@@ -2409,8 +2690,12 @@
       <c r="G72" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H72" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('CloudERA ', 7, 70);</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>85</v>
       </c>
@@ -2418,7 +2703,7 @@
         <v>107</v>
       </c>
       <c r="D73" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Cognos Bi</v>
       </c>
       <c r="E73" t="s">
@@ -2430,8 +2715,12 @@
       <c r="G73" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H73" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Cognos Bi', 7, 71);</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>149</v>
       </c>
@@ -2439,7 +2728,7 @@
         <v>107</v>
       </c>
       <c r="D74" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Csharp</v>
       </c>
       <c r="E74" t="s">
@@ -2451,8 +2740,12 @@
       <c r="G74" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H74" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Csharp', 7, 72);</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>145</v>
       </c>
@@ -2460,7 +2753,7 @@
         <v>107</v>
       </c>
       <c r="D75" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Css</v>
       </c>
       <c r="E75" t="s">
@@ -2472,8 +2765,12 @@
       <c r="G75" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H75" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Css', 7, 73);</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>9</v>
       </c>
@@ -2481,7 +2778,7 @@
         <v>107</v>
       </c>
       <c r="D76" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Cybersecurity </v>
       </c>
       <c r="E76" t="s">
@@ -2493,8 +2790,12 @@
       <c r="G76" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H76" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Cybersecurity ', 7, 74);</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>152</v>
       </c>
@@ -2502,7 +2803,7 @@
         <v>107</v>
       </c>
       <c r="D77" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Data Analysis</v>
       </c>
       <c r="E77" t="s">
@@ -2514,8 +2815,12 @@
       <c r="G77" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H77" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Data Analysis', 7, 75);</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
         <v>127</v>
       </c>
@@ -2523,7 +2828,7 @@
         <v>107</v>
       </c>
       <c r="D78" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Data Analyst</v>
       </c>
       <c r="E78" t="s">
@@ -2535,8 +2840,12 @@
       <c r="G78" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H78" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Data Analyst', 7, 76);</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>153</v>
       </c>
@@ -2544,7 +2853,7 @@
         <v>107</v>
       </c>
       <c r="D79" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Data Analytics</v>
       </c>
       <c r="E79" t="s">
@@ -2556,8 +2865,12 @@
       <c r="G79" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H79" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Data Analytics', 7, 77);</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>61</v>
       </c>
@@ -2565,7 +2878,7 @@
         <v>107</v>
       </c>
       <c r="D80" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Data Engineering </v>
       </c>
       <c r="E80" t="s">
@@ -2577,8 +2890,12 @@
       <c r="G80" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H80" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Data Engineering ', 7, 78);</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>157</v>
       </c>
@@ -2586,7 +2903,7 @@
         <v>107</v>
       </c>
       <c r="D81" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Data Governance</v>
       </c>
       <c r="E81" t="s">
@@ -2598,8 +2915,12 @@
       <c r="G81" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H81" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Data Governance', 7, 79);</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
         <v>142</v>
       </c>
@@ -2607,7 +2928,7 @@
         <v>107</v>
       </c>
       <c r="D82" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Data Store</v>
       </c>
       <c r="E82" t="s">
@@ -2619,8 +2940,12 @@
       <c r="G82" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H82" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Data Store', 7, 80);</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>28</v>
       </c>
@@ -2628,7 +2953,7 @@
         <v>107</v>
       </c>
       <c r="D83" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Datascience</v>
       </c>
       <c r="E83" t="s">
@@ -2640,8 +2965,12 @@
       <c r="G83" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H83" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Datascience', 7, 81);</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>88</v>
       </c>
@@ -2649,7 +2978,7 @@
         <v>107</v>
       </c>
       <c r="D84" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>DataStage </v>
       </c>
       <c r="E84" t="s">
@@ -2661,8 +2990,12 @@
       <c r="G84" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H84" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('DataStage ', 7, 82);</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>27</v>
       </c>
@@ -2670,7 +3003,7 @@
         <v>107</v>
       </c>
       <c r="D85" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Devops</v>
       </c>
       <c r="E85" t="s">
@@ -2682,8 +3015,12 @@
       <c r="G85" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H85" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Devops', 7, 83);</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>8</v>
       </c>
@@ -2691,7 +3028,7 @@
         <v>107</v>
       </c>
       <c r="D86" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>DevOps + AWS </v>
       </c>
       <c r="E86" t="s">
@@ -2703,8 +3040,12 @@
       <c r="G86" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H86" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('DevOps + AWS ', 7, 84);</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
         <v>82</v>
       </c>
@@ -2712,7 +3053,7 @@
         <v>107</v>
       </c>
       <c r="D87" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">Django </v>
       </c>
       <c r="E87" t="s">
@@ -2724,8 +3065,12 @@
       <c r="G87" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H87" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Django ', 7, 85);</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>103</v>
       </c>
@@ -2733,7 +3078,7 @@
         <v>107</v>
       </c>
       <c r="D88" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Docker</v>
       </c>
       <c r="E88" t="s">
@@ -2745,8 +3090,12 @@
       <c r="G88" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H88" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Docker', 7, 86);</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>154</v>
       </c>
@@ -2754,7 +3103,7 @@
         <v>107</v>
       </c>
       <c r="D89" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Dot Net Core</v>
       </c>
       <c r="E89" t="s">
@@ -2766,8 +3115,12 @@
       <c r="G89" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H89" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Dot Net Core', 7, 87);</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>83</v>
       </c>
@@ -2775,7 +3128,7 @@
         <v>107</v>
       </c>
       <c r="D90" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>DOT NET </v>
       </c>
       <c r="E90" t="s">
@@ -2787,8 +3140,12 @@
       <c r="G90" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H90" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('DOT NET ', 7, 88);</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>10</v>
       </c>
@@ -2796,7 +3153,7 @@
         <v>107</v>
       </c>
       <c r="D91" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Drupal </v>
       </c>
       <c r="E91" t="s">
@@ -2808,8 +3165,12 @@
       <c r="G91" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H91" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Drupal ', 7, 89);</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
         <v>117</v>
       </c>
@@ -2817,7 +3178,7 @@
         <v>107</v>
       </c>
       <c r="D92" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">Flask </v>
       </c>
       <c r="E92" t="s">
@@ -2829,8 +3190,12 @@
       <c r="G92" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H92" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Flask ', 7, 90);</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>22</v>
       </c>
@@ -2838,7 +3203,7 @@
         <v>107</v>
       </c>
       <c r="D93" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GCP</v>
       </c>
       <c r="E93" t="s">
@@ -2850,8 +3215,12 @@
       <c r="G93" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H93" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('GCP', 7, 91);</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="s">
         <v>119</v>
       </c>
@@ -2859,7 +3228,7 @@
         <v>107</v>
       </c>
       <c r="D94" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GIT</v>
       </c>
       <c r="E94" t="s">
@@ -2871,8 +3240,12 @@
       <c r="G94" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H94" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('GIT', 7, 92);</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>156</v>
       </c>
@@ -2880,7 +3253,7 @@
         <v>107</v>
       </c>
       <c r="D95" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Golang</v>
       </c>
       <c r="E95" t="s">
@@ -2892,8 +3265,12 @@
       <c r="G95" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H95" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Golang', 7, 93);</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>143</v>
       </c>
@@ -2901,7 +3278,7 @@
         <v>107</v>
       </c>
       <c r="D96" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Hadoop </v>
       </c>
       <c r="E96" t="s">
@@ -2913,8 +3290,12 @@
       <c r="G96" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H96" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Hadoop ', 7, 94);</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>146</v>
       </c>
@@ -2922,7 +3303,7 @@
         <v>107</v>
       </c>
       <c r="D97" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HTML</v>
       </c>
       <c r="E97" t="s">
@@ -2934,8 +3315,12 @@
       <c r="G97" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H97" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('HTML', 7, 95);</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>84</v>
       </c>
@@ -2943,7 +3328,7 @@
         <v>107</v>
       </c>
       <c r="D98" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Informatica</v>
       </c>
       <c r="E98" t="s">
@@ -2955,8 +3340,12 @@
       <c r="G98" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H98" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Informatica', 7, 96);</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>125</v>
       </c>
@@ -2964,7 +3353,7 @@
         <v>107</v>
       </c>
       <c r="D99" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Informatica Power Center</v>
       </c>
       <c r="E99" t="s">
@@ -2976,8 +3365,12 @@
       <c r="G99" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H99" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Informatica Power Center', 7, 97);</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>95</v>
       </c>
@@ -2985,7 +3378,7 @@
         <v>107</v>
       </c>
       <c r="D100" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>IOS </v>
       </c>
       <c r="E100" t="s">
@@ -2997,8 +3390,12 @@
       <c r="G100" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H100" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('IOS ', 7, 98);</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>29</v>
       </c>
@@ -3006,7 +3403,7 @@
         <v>107</v>
       </c>
       <c r="D101" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>IOT</v>
       </c>
       <c r="E101" t="s">
@@ -3018,8 +3415,12 @@
       <c r="G101" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H101" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('IOT', 7, 99);</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>99</v>
       </c>
@@ -3027,7 +3428,7 @@
         <v>107</v>
       </c>
       <c r="D102" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Java Full Stack</v>
       </c>
       <c r="E102" t="s">
@@ -3039,8 +3440,12 @@
       <c r="G102" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H102" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Java Full Stack', 7, 100);</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="4" t="s">
         <v>123</v>
       </c>
@@ -3048,7 +3453,7 @@
         <v>107</v>
       </c>
       <c r="D103" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Jenkins</v>
       </c>
       <c r="E103" t="s">
@@ -3060,8 +3465,12 @@
       <c r="G103" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H103" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Jenkins', 7, 101);</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>126</v>
       </c>
@@ -3069,7 +3478,7 @@
         <v>107</v>
       </c>
       <c r="D104" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Jira admin </v>
       </c>
       <c r="E104" t="s">
@@ -3081,8 +3490,12 @@
       <c r="G104" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H104" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Jira admin ', 7, 102);</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>15</v>
       </c>
@@ -3090,7 +3503,7 @@
         <v>107</v>
       </c>
       <c r="D105" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">Juniper </v>
       </c>
       <c r="E105" t="s">
@@ -3102,8 +3515,12 @@
       <c r="G105" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H105" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Juniper ', 7, 103);</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>24</v>
       </c>
@@ -3111,7 +3528,7 @@
         <v>107</v>
       </c>
       <c r="D106" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Kafka </v>
       </c>
       <c r="E106" t="s">
@@ -3123,8 +3540,12 @@
       <c r="G106" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H106" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Kafka ', 7, 104);</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>104</v>
       </c>
@@ -3132,7 +3553,7 @@
         <v>107</v>
       </c>
       <c r="D107" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Kubernetes - Admin</v>
       </c>
       <c r="E107" t="s">
@@ -3144,8 +3565,12 @@
       <c r="G107" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H107" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Kubernetes - Admin', 7, 105);</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>75</v>
       </c>
@@ -3153,7 +3578,7 @@
         <v>107</v>
       </c>
       <c r="D108" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Kubernetes - Developer</v>
       </c>
       <c r="E108" t="s">
@@ -3165,8 +3590,12 @@
       <c r="G108" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H108" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Kubernetes - Developer', 7, 106);</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>129</v>
       </c>
@@ -3174,7 +3603,7 @@
         <v>107</v>
       </c>
       <c r="D109" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Linux</v>
       </c>
       <c r="E109" t="s">
@@ -3186,8 +3615,12 @@
       <c r="G109" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H109" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Linux', 7, 107);</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="4" t="s">
         <v>122</v>
       </c>
@@ -3195,7 +3628,7 @@
         <v>107</v>
       </c>
       <c r="D110" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Maven</v>
       </c>
       <c r="E110" t="s">
@@ -3207,8 +3640,12 @@
       <c r="G110" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H110" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Maven', 7, 108);</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="4" t="s">
         <v>76</v>
       </c>
@@ -3216,7 +3653,7 @@
         <v>107</v>
       </c>
       <c r="D111" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>MicroStratogy</v>
       </c>
       <c r="E111" t="s">
@@ -3228,8 +3665,12 @@
       <c r="G111" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H111" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('MicroStratogy', 7, 109);</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>69</v>
       </c>
@@ -3237,7 +3678,7 @@
         <v>107</v>
       </c>
       <c r="D112" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>MSBI</v>
       </c>
       <c r="E112" t="s">
@@ -3249,8 +3690,12 @@
       <c r="G112" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H112" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('MSBI', 7, 110);</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>19</v>
       </c>
@@ -3258,7 +3703,7 @@
         <v>107</v>
       </c>
       <c r="D113" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Mulesoft</v>
       </c>
       <c r="E113" t="s">
@@ -3270,8 +3715,12 @@
       <c r="G113" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H113" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Mulesoft', 7, 111);</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>130</v>
       </c>
@@ -3279,7 +3728,7 @@
         <v>107</v>
       </c>
       <c r="D114" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Networking</v>
       </c>
       <c r="E114" t="s">
@@ -3291,8 +3740,12 @@
       <c r="G114" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H114" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Networking', 7, 112);</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="4" t="s">
         <v>116</v>
       </c>
@@ -3300,7 +3753,7 @@
         <v>107</v>
       </c>
       <c r="D115" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>NumPy</v>
       </c>
       <c r="E115" t="s">
@@ -3312,8 +3765,12 @@
       <c r="G115" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H115" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('NumPy', 7, 113);</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>105</v>
       </c>
@@ -3321,7 +3778,7 @@
         <v>107</v>
       </c>
       <c r="D116" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>OBI EE</v>
       </c>
       <c r="E116" t="s">
@@ -3333,8 +3790,12 @@
       <c r="G116" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H116" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('OBI EE', 7, 114);</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="4" t="s">
         <v>141</v>
       </c>
@@ -3342,7 +3803,7 @@
         <v>107</v>
       </c>
       <c r="D117" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">Oracle </v>
       </c>
       <c r="E117" t="s">
@@ -3354,8 +3815,12 @@
       <c r="G117" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H117" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Oracle ', 7, 115);</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>162</v>
       </c>
@@ -3363,7 +3828,7 @@
         <v>107</v>
       </c>
       <c r="D118" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Oracle Cloud</v>
       </c>
       <c r="E118" t="s">
@@ -3375,8 +3840,12 @@
       <c r="G118" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H118" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Oracle Cloud', 7, 116);</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>71</v>
       </c>
@@ -3384,7 +3853,7 @@
         <v>107</v>
       </c>
       <c r="D119" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Oracle DBA</v>
       </c>
       <c r="E119" t="s">
@@ -3396,8 +3865,12 @@
       <c r="G119" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H119" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Oracle DBA', 7, 117);</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>159</v>
       </c>
@@ -3405,7 +3878,7 @@
         <v>107</v>
       </c>
       <c r="D120" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Oracle Dba</v>
       </c>
       <c r="E120" t="s">
@@ -3417,8 +3890,12 @@
       <c r="G120" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H120" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Oracle Dba', 7, 118);</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>161</v>
       </c>
@@ -3426,7 +3903,7 @@
         <v>107</v>
       </c>
       <c r="D121" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Oracle Ebs</v>
       </c>
       <c r="E121" t="s">
@@ -3438,8 +3915,12 @@
       <c r="G121" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H121" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Oracle Ebs', 7, 119);</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>160</v>
       </c>
@@ -3447,7 +3928,7 @@
         <v>107</v>
       </c>
       <c r="D122" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Oracle Pl/Sql</v>
       </c>
       <c r="E122" t="s">
@@ -3459,8 +3940,12 @@
       <c r="G122" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H122" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Oracle Pl/Sql', 7, 120);</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>1</v>
       </c>
@@ -3468,7 +3953,7 @@
         <v>107</v>
       </c>
       <c r="D123" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Oracle </v>
       </c>
       <c r="E123" t="s">
@@ -3480,8 +3965,12 @@
       <c r="G123" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H123" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Oracle ', 7, 121);</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>2</v>
       </c>
@@ -3489,7 +3978,7 @@
         <v>107</v>
       </c>
       <c r="D124" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Palo Alto </v>
       </c>
       <c r="E124" t="s">
@@ -3501,8 +3990,12 @@
       <c r="G124" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="125" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H124" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Palo Alto ', 7, 122);</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="4" t="s">
         <v>115</v>
       </c>
@@ -3510,7 +4003,7 @@
         <v>107</v>
       </c>
       <c r="D125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Pandas</v>
       </c>
       <c r="E125" t="s">
@@ -3522,8 +4015,12 @@
       <c r="G125" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="126" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H125" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Pandas', 7, 123);</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>158</v>
       </c>
@@ -3531,7 +4028,7 @@
         <v>107</v>
       </c>
       <c r="D126" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Pega Prpc</v>
       </c>
       <c r="E126" t="s">
@@ -3543,8 +4040,12 @@
       <c r="G126" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H126" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Pega Prpc', 7, 124);</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>11</v>
       </c>
@@ -3552,7 +4053,7 @@
         <v>107</v>
       </c>
       <c r="D127" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Pega </v>
       </c>
       <c r="E127" t="s">
@@ -3564,8 +4065,12 @@
       <c r="G127" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H127" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Pega ', 7, 125);</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>101</v>
       </c>
@@ -3573,7 +4078,7 @@
         <v>107</v>
       </c>
       <c r="D128" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>PeopleSoft</v>
       </c>
       <c r="E128" t="s">
@@ -3585,8 +4090,12 @@
       <c r="G128" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H128" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('PeopleSoft', 7, 126);</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>59</v>
       </c>
@@ -3594,7 +4103,7 @@
         <v>107</v>
       </c>
       <c r="D129" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>PHP </v>
       </c>
       <c r="E129" t="s">
@@ -3606,8 +4115,12 @@
       <c r="G129" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="130" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H129" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('PHP ', 7, 127);</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>164</v>
       </c>
@@ -3615,7 +4128,7 @@
         <v>107</v>
       </c>
       <c r="D130" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Power Automate</v>
       </c>
       <c r="E130" t="s">
@@ -3627,8 +4140,12 @@
       <c r="G130" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="131" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H130" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Power Automate', 7, 128);</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>67</v>
       </c>
@@ -3636,7 +4153,7 @@
         <v>107</v>
       </c>
       <c r="D131" t="str">
-        <f t="shared" ref="D131:D165" si="2">A131</f>
+        <f t="shared" ref="D131:D165" si="4">A131</f>
         <v>Power BI</v>
       </c>
       <c r="E131" t="s">
@@ -3648,8 +4165,12 @@
       <c r="G131" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="132" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H131" t="str">
+        <f t="shared" ref="H131:H165" si="5">_xlfn.CONCAT(C131,D131,E131,F131,G131)</f>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Power BI', 7, 129);</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>163</v>
       </c>
@@ -3657,7 +4178,7 @@
         <v>107</v>
       </c>
       <c r="D132" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>Powerpoint</v>
       </c>
       <c r="E132" t="s">
@@ -3669,8 +4190,12 @@
       <c r="G132" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="133" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H132" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Powerpoint', 7, 130);</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>20</v>
       </c>
@@ -3678,7 +4203,7 @@
         <v>107</v>
       </c>
       <c r="D133" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>Powershell</v>
       </c>
       <c r="E133" t="s">
@@ -3690,8 +4215,12 @@
       <c r="G133" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="134" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H133" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Powershell', 7, 131);</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>25</v>
       </c>
@@ -3699,7 +4228,7 @@
         <v>107</v>
       </c>
       <c r="D134" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>Pyspark</v>
       </c>
       <c r="E134" t="s">
@@ -3711,8 +4240,12 @@
       <c r="G134" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H134" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Pyspark', 7, 132);</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>74</v>
       </c>
@@ -3720,7 +4253,7 @@
         <v>107</v>
       </c>
       <c r="D135" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>Python</v>
       </c>
       <c r="E135" t="s">
@@ -3732,8 +4265,12 @@
       <c r="G135" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H135" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Python', 7, 133);</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>165</v>
       </c>
@@ -3741,7 +4278,7 @@
         <v>107</v>
       </c>
       <c r="D136" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>Python Django</v>
       </c>
       <c r="E136" t="s">
@@ -3753,8 +4290,12 @@
       <c r="G136" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="137" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H136" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Python Django', 7, 134);</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>68</v>
       </c>
@@ -3762,7 +4303,7 @@
         <v>107</v>
       </c>
       <c r="D137" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>QlikView</v>
       </c>
       <c r="E137" t="s">
@@ -3774,8 +4315,12 @@
       <c r="G137" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="138" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H137" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('QlikView', 7, 135);</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>166</v>
       </c>
@@ -3783,7 +4328,7 @@
         <v>107</v>
       </c>
       <c r="D138" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>React Native</v>
       </c>
       <c r="E138" t="s">
@@ -3795,8 +4340,12 @@
       <c r="G138" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="139" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H138" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('React Native', 7, 136);</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>79</v>
       </c>
@@ -3804,7 +4353,7 @@
         <v>107</v>
       </c>
       <c r="D139" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>RPA- UiPath</v>
       </c>
       <c r="E139" t="s">
@@ -3816,8 +4365,12 @@
       <c r="G139" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="140" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H139" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('RPA- UiPath', 7, 137);</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>80</v>
       </c>
@@ -3825,7 +4378,7 @@
         <v>107</v>
       </c>
       <c r="D140" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>RPA-Blueprism</v>
       </c>
       <c r="E140" t="s">
@@ -3837,8 +4390,12 @@
       <c r="G140" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H140" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('RPA-Blueprism', 7, 138);</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>97</v>
       </c>
@@ -3846,7 +4403,7 @@
         <v>107</v>
       </c>
       <c r="D141" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>Sailpoint </v>
       </c>
       <c r="E141" t="s">
@@ -3858,8 +4415,12 @@
       <c r="G141" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="142" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H141" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Sailpoint ', 7, 139);</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>93</v>
       </c>
@@ -3867,7 +4428,7 @@
         <v>107</v>
       </c>
       <c r="D142" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>Salesforce Developer </v>
       </c>
       <c r="E142" t="s">
@@ -3879,8 +4440,12 @@
       <c r="G142" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="143" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H142" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Salesforce Developer ', 7, 140);</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>106</v>
       </c>
@@ -3888,7 +4453,7 @@
         <v>107</v>
       </c>
       <c r="D143" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>Salesforce  Admin</v>
       </c>
       <c r="E143" t="s">
@@ -3900,8 +4465,12 @@
       <c r="G143" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="144" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H143" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Salesforce  Admin', 7, 141);</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>92</v>
       </c>
@@ -3909,7 +4478,7 @@
         <v>107</v>
       </c>
       <c r="D144" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>SAP</v>
       </c>
       <c r="E144" t="s">
@@ -3921,8 +4490,12 @@
       <c r="G144" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="145" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H144" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('SAP', 7, 142);</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>3</v>
       </c>
@@ -3930,7 +4503,7 @@
         <v>107</v>
       </c>
       <c r="D145" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>SAS </v>
       </c>
       <c r="E145" t="s">
@@ -3942,8 +4515,12 @@
       <c r="G145" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="146" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H145" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('SAS ', 7, 143);</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="4" t="s">
         <v>78</v>
       </c>
@@ -3951,7 +4528,7 @@
         <v>107</v>
       </c>
       <c r="D146" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>Selenium</v>
       </c>
       <c r="E146" t="s">
@@ -3963,8 +4540,12 @@
       <c r="G146" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="147" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H146" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Selenium', 7, 144);</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>17</v>
       </c>
@@ -3972,7 +4553,7 @@
         <v>107</v>
       </c>
       <c r="D147" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>ServiceNow Admin</v>
       </c>
       <c r="E147" t="s">
@@ -3984,8 +4565,12 @@
       <c r="G147" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="148" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H147" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('ServiceNow Admin', 7, 145);</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>18</v>
       </c>
@@ -3993,7 +4578,7 @@
         <v>107</v>
       </c>
       <c r="D148" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>ServiceNow Developer </v>
       </c>
       <c r="E148" t="s">
@@ -4005,8 +4590,12 @@
       <c r="G148" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="149" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H148" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('ServiceNow Developer ', 7, 146);</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="4" t="s">
         <v>77</v>
       </c>
@@ -4014,7 +4603,7 @@
         <v>107</v>
       </c>
       <c r="D149" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>Share Point</v>
       </c>
       <c r="E149" t="s">
@@ -4026,8 +4615,12 @@
       <c r="G149" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="150" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H149" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Share Point', 7, 147);</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>21</v>
       </c>
@@ -4035,7 +4628,7 @@
         <v>107</v>
       </c>
       <c r="D150" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>Snowflake</v>
       </c>
       <c r="E150" t="s">
@@ -4047,8 +4640,12 @@
       <c r="G150" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="151" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H150" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Snowflake', 7, 148);</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>167</v>
       </c>
@@ -4056,7 +4653,7 @@
         <v>107</v>
       </c>
       <c r="D151" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>Spark</v>
       </c>
       <c r="E151" t="s">
@@ -4068,8 +4665,12 @@
       <c r="G151" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="152" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H151" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Spark', 7, 149);</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>6</v>
       </c>
@@ -4077,7 +4678,7 @@
         <v>107</v>
       </c>
       <c r="D152" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>Splunk </v>
       </c>
       <c r="E152" t="s">
@@ -4089,8 +4690,12 @@
       <c r="G152" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="153" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H152" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Splunk ', 7, 150);</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>150</v>
       </c>
@@ -4098,7 +4703,7 @@
         <v>107</v>
       </c>
       <c r="D153" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>Spring Boot</v>
       </c>
       <c r="E153" t="s">
@@ -4110,8 +4715,12 @@
       <c r="G153" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="154" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H153" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Spring Boot', 7, 151);</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="4" t="s">
         <v>140</v>
       </c>
@@ -4119,7 +4728,7 @@
         <v>107</v>
       </c>
       <c r="D154" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>SQL</v>
       </c>
       <c r="E154" t="s">
@@ -4131,8 +4740,12 @@
       <c r="G154" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="155" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H154" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('SQL', 7, 152);</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>102</v>
       </c>
@@ -4140,7 +4753,7 @@
         <v>107</v>
       </c>
       <c r="D155" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>Sql dba</v>
       </c>
       <c r="E155" t="s">
@@ -4152,8 +4765,12 @@
       <c r="G155" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="156" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H155" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Sql dba', 7, 153);</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>131</v>
       </c>
@@ -4161,7 +4778,7 @@
         <v>107</v>
       </c>
       <c r="D156" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>System Administrator</v>
       </c>
       <c r="E156" t="s">
@@ -4173,8 +4790,12 @@
       <c r="G156" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="157" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H156" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('System Administrator', 7, 154);</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>26</v>
       </c>
@@ -4182,7 +4803,7 @@
         <v>107</v>
       </c>
       <c r="D157" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>Tableau</v>
       </c>
       <c r="E157" t="s">
@@ -4194,8 +4815,12 @@
       <c r="G157" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="158" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H157" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Tableau', 7, 155);</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>86</v>
       </c>
@@ -4203,7 +4828,7 @@
         <v>107</v>
       </c>
       <c r="D158" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>Teradata</v>
       </c>
       <c r="E158" t="s">
@@ -4215,8 +4840,12 @@
       <c r="G158" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="159" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H158" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Teradata', 7, 156);</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="4" t="s">
         <v>139</v>
       </c>
@@ -4224,7 +4853,7 @@
         <v>107</v>
       </c>
       <c r="D159" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>Terraform</v>
       </c>
       <c r="E159" t="s">
@@ -4236,8 +4865,12 @@
       <c r="G159" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="160" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H159" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Terraform', 7, 157);</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>89</v>
       </c>
@@ -4245,7 +4878,7 @@
         <v>107</v>
       </c>
       <c r="D160" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>Tibco</v>
       </c>
       <c r="E160" t="s">
@@ -4257,8 +4890,12 @@
       <c r="G160" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="161" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H160" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Tibco', 7, 158);</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>5</v>
       </c>
@@ -4266,7 +4903,7 @@
         <v>107</v>
       </c>
       <c r="D161" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>TOGAF </v>
       </c>
       <c r="E161" t="s">
@@ -4278,8 +4915,12 @@
       <c r="G161" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="162" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H161" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('TOGAF ', 7, 159);</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>128</v>
       </c>
@@ -4287,7 +4928,7 @@
         <v>107</v>
       </c>
       <c r="D162" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>UI/UX</v>
       </c>
       <c r="E162" t="s">
@@ -4299,8 +4940,12 @@
       <c r="G162" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="163" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H162" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('UI/UX', 7, 160);</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>100</v>
       </c>
@@ -4308,7 +4953,7 @@
         <v>107</v>
       </c>
       <c r="D163" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>WebLogic </v>
       </c>
       <c r="E163" t="s">
@@ -4320,8 +4965,12 @@
       <c r="G163" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="164" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H163" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('WebLogic ', 7, 161);</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>91</v>
       </c>
@@ -4329,7 +4978,7 @@
         <v>107</v>
       </c>
       <c r="D164" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>Workday</v>
       </c>
       <c r="E164" t="s">
@@ -4341,8 +4990,12 @@
       <c r="G164" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="165" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H164" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Workday', 7, 162);</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>12</v>
       </c>
@@ -4350,7 +5003,7 @@
         <v>107</v>
       </c>
       <c r="D165" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>Workday HCM </v>
       </c>
       <c r="E165" t="s">
@@ -4361,6 +5014,10 @@
       </c>
       <c r="G165" t="s">
         <v>109</v>
+      </c>
+      <c r="H165" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO [SpecificationAttributeOption] ( [Name], [SpecificationAttributeId], [DisplayOrder]) VALUES ('Workday HCM ', 7, 163);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sql scripts and technology list excel updated
</commit_message>
<xml_diff>
--- a/DocumentsAndScripts/Technology List.xlsx
+++ b/DocumentsAndScripts/Technology List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venroja\source\repos\sateeshmunagala\nopCommerce\DocumentsAndScripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nopcommerce\sateeshmunagala\nopCommerce\DocumentsAndScripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506C9775-1680-400D-ADA2-FFE2EB344513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4D4BC3-F436-4D7A-8CE9-7C47BF481327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -901,8 +901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C142" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H165"/>
+    <sheetView tabSelected="1" topLeftCell="B140" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H165" sqref="H165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -910,8 +910,7 @@
     <col min="1" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="98" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="128.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5034,7 +5033,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0819E9B8-05A7-4F50-8DBE-11C3FF5827B7}">
   <dimension ref="A1:A165"/>
   <sheetViews>
-    <sheetView topLeftCell="A147" workbookViewId="0">
+    <sheetView topLeftCell="A132" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A165"/>
     </sheetView>
   </sheetViews>

</xml_diff>